<commit_message>
ændret substantielt i methods.py, sorting script, robot simulator, measurement excel dokument og simulatorTests
</commit_message>
<xml_diff>
--- a/Ressourcer/Measure.xlsx
+++ b/Ressourcer/Measure.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="15120" windowHeight="4695"/>
@@ -11,12 +11,12 @@
     <sheet name="Ark2" sheetId="2" r:id="rId2"/>
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>Rød</t>
   </si>
@@ -124,13 +124,97 @@
   </si>
   <si>
     <t>Masse g</t>
+  </si>
+  <si>
+    <t>"-35939 -201917 222128 -91577 174695"</t>
+  </si>
+  <si>
+    <t>DropPosition</t>
+  </si>
+  <si>
+    <t>BoxLine</t>
+  </si>
+  <si>
+    <t>"-34426 -197352 113102 -94767 175519"</t>
+  </si>
+  <si>
+    <t>"-34361 -240018 100770 -87921 177096"</t>
+  </si>
+  <si>
+    <t>"-34233 -296984 107400 -87885 178422"</t>
+  </si>
+  <si>
+    <t>(-35662,-371994,111897,-91433,179068)</t>
+  </si>
+  <si>
+    <t>(-110514,-196048,113067,-91146,154444)</t>
+  </si>
+  <si>
+    <t>(-110688,-196356,193476,-91146,154444)</t>
+  </si>
+  <si>
+    <t>(-114921,-244110,102712,-91039,158028)</t>
+  </si>
+  <si>
+    <t>(-115072,-299517,117515,-90896,162007)</t>
+  </si>
+  <si>
+    <t>(-115176,-359434,116646,-90824,164838)</t>
+  </si>
+  <si>
+    <t>(115987,-204580,115036,-90752,211684)</t>
+  </si>
+  <si>
+    <t>(116082,-204747,176224,-90752,211684)</t>
+  </si>
+  <si>
+    <t>(116645,-259437,114312,-90609,208853)</t>
+  </si>
+  <si>
+    <t>(116873,-311507,114186,-90573,205125)</t>
+  </si>
+  <si>
+    <t>(117706,-376552,109322,-90501,201792)</t>
+  </si>
+  <si>
+    <t>(40570,-196648,107766,-90071,195125)</t>
+  </si>
+  <si>
+    <t>(40594,-196765,197469,-90035,195125)</t>
+  </si>
+  <si>
+    <t>(40705,-254173,122044,-90000,192473)</t>
+  </si>
+  <si>
+    <t>(40082,-319053,103088,-90000,190286)</t>
+  </si>
+  <si>
+    <t>(40123,-374801,102765,-90035,189318)</t>
+  </si>
+  <si>
+    <t>(-228374,54397,113627,-88279,-99175)</t>
+  </si>
+  <si>
+    <t>(-228776,156978,113499,-88243,-122759)</t>
+  </si>
+  <si>
+    <t>(-229004,262880,113265,-88207,-137240)</t>
+  </si>
+  <si>
+    <t>(-228408,363383,114639,-88172,-146200)</t>
+  </si>
+  <si>
+    <t>(-228005,216893,255920,-88172,-131469)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="173" formatCode="#,##0.000"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,10 +225,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -170,8 +258,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -182,9 +270,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kontortema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kontor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -222,7 +310,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kontor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -292,7 +380,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kontor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -466,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -481,9 +569,11 @@
     <col min="5" max="5" width="20.42578125" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="35.42578125" customWidth="1"/>
+    <col min="9" max="9" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,8 +595,14 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -523,11 +619,21 @@
         <f>B2*C2*D2</f>
         <v>411600</v>
       </c>
-      <c r="F2" s="2">
-        <v>156926</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="F2" s="3">
+        <v>156.92599999999999</v>
+      </c>
+      <c r="G2">
+        <f>F2/E2*1000</f>
+        <v>0.38125850340136053</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -544,11 +650,21 @@
         <f>B3*C3*D3</f>
         <v>390432</v>
       </c>
-      <c r="F3" s="2">
-        <v>150080</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="F3" s="3">
+        <v>150.08000000000001</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G30" si="0">F3/E3*1000</f>
+        <v>0.38439472174411937</v>
+      </c>
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -565,11 +681,21 @@
         <f>B4*C4*D4</f>
         <v>343000</v>
       </c>
-      <c r="F4" s="2">
-        <v>130533</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="F4" s="3">
+        <v>130.53299999999999</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0.38056268221574341</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -586,11 +712,21 @@
         <f>B5*C5*D5</f>
         <v>274400</v>
       </c>
-      <c r="F5" s="2">
-        <v>106095</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="F5" s="3">
+        <v>106.095</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>0.38664358600583087</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -607,16 +743,24 @@
         <f>B6*C6*D6</f>
         <v>209440</v>
       </c>
-      <c r="F6" s="2">
-        <v>84590</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="F6" s="3">
+        <v>84.59</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0.40388655462184875</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -633,11 +777,21 @@
         <f>B8*C8*D8</f>
         <v>411600</v>
       </c>
-      <c r="F8" s="2">
-        <v>196027</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="F8" s="3">
+        <v>196.02699999999999</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0.47625607385811464</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -654,11 +808,21 @@
         <f>B9*C9*D9</f>
         <v>390432</v>
       </c>
-      <c r="F9" s="2">
-        <v>188207</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="F9" s="3">
+        <v>188.20699999999999</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0.48204809032046553</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -675,11 +839,21 @@
         <f>B10*C10*D10</f>
         <v>343000</v>
       </c>
-      <c r="F10" s="2">
-        <v>162791</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="F10" s="3">
+        <v>162.791</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0.47460932944606415</v>
+      </c>
+      <c r="H10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -696,11 +870,21 @@
         <f>B11*C11*D11</f>
         <v>274400</v>
       </c>
-      <c r="F11" s="2">
-        <v>132488</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="F11" s="3">
+        <v>132.488</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0.4828279883381924</v>
+      </c>
+      <c r="H11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -717,16 +901,24 @@
         <f>B12*C12*D12</f>
         <v>219520</v>
       </c>
-      <c r="F12" s="2">
-        <v>105118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="F12" s="3">
+        <v>105.11799999999999</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0.47885386297376092</v>
+      </c>
+      <c r="H12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -743,11 +935,21 @@
         <f>B14*C14*D14</f>
         <v>411600</v>
       </c>
-      <c r="F14" s="2">
-        <v>127601</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="F14" s="3">
+        <v>127.601</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0.31001214771622937</v>
+      </c>
+      <c r="H14" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -764,11 +966,21 @@
         <f>B15*C15*D15</f>
         <v>343000</v>
       </c>
-      <c r="F15" s="2">
-        <v>104140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="F15" s="3">
+        <v>104.14</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0.30361516034985425</v>
+      </c>
+      <c r="H15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -785,11 +997,21 @@
         <f>B16*C16*D16</f>
         <v>270480</v>
       </c>
-      <c r="F16" s="2">
-        <v>84590</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="F16" s="3">
+        <v>84.59</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0.31274031351671105</v>
+      </c>
+      <c r="H16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -806,21 +1028,33 @@
         <f>B17*C17*D17</f>
         <v>219520</v>
       </c>
-      <c r="F17" s="2">
-        <v>66017</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="F17" s="3">
+        <v>66.016999999999996</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>0.30073341836734691</v>
+      </c>
+      <c r="H17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -837,11 +1071,21 @@
         <f>B20*C20*D20</f>
         <v>411600</v>
       </c>
-      <c r="F20" s="2">
-        <v>105118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="F20" s="3">
+        <v>105.11799999999999</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>0.25538872691933917</v>
+      </c>
+      <c r="H20" t="s">
+        <v>49</v>
+      </c>
+      <c r="I20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -858,11 +1102,21 @@
         <f>B21*C21*D21</f>
         <v>390432</v>
       </c>
-      <c r="F21" s="2">
-        <v>102185</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="F21" s="3">
+        <v>102.185</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>0.26172291205638887</v>
+      </c>
+      <c r="H21" t="s">
+        <v>49</v>
+      </c>
+      <c r="I21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -875,15 +1129,25 @@
       <c r="D22">
         <v>70</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <f>B22*C22*D22</f>
         <v>343000</v>
       </c>
-      <c r="F22" s="2">
-        <v>81657</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="F22" s="3">
+        <v>76.770185728300007</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>0.22381978346443152</v>
+      </c>
+      <c r="H22" t="s">
+        <v>49</v>
+      </c>
+      <c r="I22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -900,11 +1164,21 @@
         <f>B23*C23*D23</f>
         <v>270480</v>
       </c>
-      <c r="F23" s="2">
-        <v>71882</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="F23" s="3">
+        <v>71.882000000000005</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>0.26575717243419111</v>
+      </c>
+      <c r="H23" t="s">
+        <v>49</v>
+      </c>
+      <c r="I23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -921,16 +1195,24 @@
         <f>B24*C24*D24</f>
         <v>219520</v>
       </c>
-      <c r="F24" s="2">
-        <v>57218</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="F24" s="3">
+        <v>57.218000000000004</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>0.26065051020408164</v>
+      </c>
+      <c r="H24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -947,11 +1229,21 @@
         <f>B26*C26*D26</f>
         <v>411600</v>
       </c>
-      <c r="F26" s="2">
-        <v>240015</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="F26" s="3">
+        <v>240.01499999999999</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>0.58312682215743439</v>
+      </c>
+      <c r="H26" t="s">
+        <v>62</v>
+      </c>
+      <c r="I26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -968,11 +1260,21 @@
         <f>B27*C27*D27</f>
         <v>390432</v>
       </c>
-      <c r="F27" s="2">
-        <v>231217</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="F27" s="3">
+        <v>231.21700000000001</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>0.59220811818703389</v>
+      </c>
+      <c r="H27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -989,11 +1291,21 @@
         <f>B28*C28*D28</f>
         <v>343000</v>
       </c>
-      <c r="F28" s="2">
-        <v>201892</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="F28" s="3">
+        <v>201.892</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>0.58860641399416913</v>
+      </c>
+      <c r="H28" t="s">
+        <v>62</v>
+      </c>
+      <c r="I28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1010,11 +1322,21 @@
         <f>B29*C29*D29</f>
         <v>270480</v>
       </c>
-      <c r="F29" s="2">
-        <v>162791</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="F29" s="3">
+        <v>162.791</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>0.60185965690624077</v>
+      </c>
+      <c r="H29" t="s">
+        <v>62</v>
+      </c>
+      <c r="I29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1031,11 +1353,16 @@
         <f>B30*C30*D30</f>
         <v>219520</v>
       </c>
-      <c r="F30" s="2">
-        <v>128578</v>
+      <c r="F30" s="3">
+        <v>128.578</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>0.58572339650145777</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1049,6 +1376,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1061,6 +1389,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ændret i methods.py sorting_script robot sqlhandler og measure
</commit_message>
<xml_diff>
--- a/Ressourcer/Measure.xlsx
+++ b/Ressourcer/Measure.xlsx
@@ -212,7 +212,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="#,##0.000"/>
+    <numFmt numFmtId="172" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -259,7 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>

<commit_message>
fjernet mange timers fra sorting script, visse er stadige nødvendige (getJawMilimeters og Weight) samt Measure
</commit_message>
<xml_diff>
--- a/Ressourcer/Measure.xlsx
+++ b/Ressourcer/Measure.xlsx
@@ -18,21 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
-    <t>Rød</t>
-  </si>
-  <si>
-    <t>Gul</t>
-  </si>
-  <si>
-    <t>Hvid</t>
-  </si>
-  <si>
-    <t>Blå</t>
-  </si>
-  <si>
-    <t>Grøn</t>
-  </si>
-  <si>
     <t>Massefylde</t>
   </si>
   <si>
@@ -205,6 +190,21 @@
   </si>
   <si>
     <t>(-228005,216893,255920,-88172,-131469)</t>
+  </si>
+  <si>
+    <t>Kategori 5</t>
+  </si>
+  <si>
+    <t>Kategori 4</t>
+  </si>
+  <si>
+    <t>Kategori 3</t>
+  </si>
+  <si>
+    <t>Kategori 2</t>
+  </si>
+  <si>
+    <t>Kategori 1</t>
   </si>
 </sst>
 </file>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -575,36 +575,36 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>70</v>
@@ -627,15 +627,15 @@
         <v>0.38125850340136053</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>84</v>
@@ -658,15 +658,15 @@
         <v>0.38439472174411937</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>70</v>
@@ -689,15 +689,15 @@
         <v>0.38056268221574341</v>
       </c>
       <c r="H4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
         <v>36</v>
-      </c>
-      <c r="I4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>56</v>
@@ -720,15 +720,15 @@
         <v>0.38664358600583087</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>56</v>
@@ -751,18 +751,18 @@
         <v>0.40388655462184875</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>70</v>
@@ -785,15 +785,15 @@
         <v>0.47625607385811464</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>84</v>
@@ -816,15 +816,15 @@
         <v>0.48204809032046553</v>
       </c>
       <c r="H9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>70</v>
@@ -847,15 +847,15 @@
         <v>0.47460932944606415</v>
       </c>
       <c r="H10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>56</v>
@@ -878,15 +878,15 @@
         <v>0.4828279883381924</v>
       </c>
       <c r="H11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>56</v>
@@ -909,18 +909,18 @@
         <v>0.47885386297376092</v>
       </c>
       <c r="H12" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>70</v>
@@ -943,15 +943,15 @@
         <v>0.31001214771622937</v>
       </c>
       <c r="H14" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>70</v>
@@ -974,15 +974,15 @@
         <v>0.30361516034985425</v>
       </c>
       <c r="H15" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B16">
         <v>70</v>
@@ -1005,15 +1005,15 @@
         <v>0.31274031351671105</v>
       </c>
       <c r="H16" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I16" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>56</v>
@@ -1036,27 +1036,27 @@
         <v>0.30073341836734691</v>
       </c>
       <c r="H17" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I17" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B20">
         <v>70</v>
@@ -1079,15 +1079,15 @@
         <v>0.25538872691933917</v>
       </c>
       <c r="H20" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I20" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B21">
         <v>84</v>
@@ -1110,15 +1110,15 @@
         <v>0.26172291205638887</v>
       </c>
       <c r="H21" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I21" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B22">
         <v>70</v>
@@ -1141,15 +1141,15 @@
         <v>0.22381978346443152</v>
       </c>
       <c r="H22" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I22" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B23">
         <v>70</v>
@@ -1172,15 +1172,15 @@
         <v>0.26575717243419111</v>
       </c>
       <c r="H23" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I23" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B24">
         <v>56</v>
@@ -1203,18 +1203,18 @@
         <v>0.26065051020408164</v>
       </c>
       <c r="H24" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B26">
         <v>70</v>
@@ -1237,15 +1237,15 @@
         <v>0.58312682215743439</v>
       </c>
       <c r="H26" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I26" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B27">
         <v>84</v>
@@ -1268,15 +1268,15 @@
         <v>0.59220811818703389</v>
       </c>
       <c r="H27" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I27" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B28">
         <v>70</v>
@@ -1299,15 +1299,15 @@
         <v>0.58860641399416913</v>
       </c>
       <c r="H28" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I28" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B29">
         <v>70</v>
@@ -1330,15 +1330,15 @@
         <v>0.60185965690624077</v>
       </c>
       <c r="H29" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I29" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B30">
         <v>56</v>

</xml_diff>